<commit_message>
MAJOR Code Update for OOTP23.
New Defense, 0-100 ratings, UI, many other things.
</commit_message>
<xml_diff>
--- a/AnalyzeOut/AnalyzeOut.xlsx
+++ b/AnalyzeOut/AnalyzeOut.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/14be9621c871c0c4/Documents/OOTP/Code/AnalyzeOut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_2B962F0BB5C56711CD3A60CB2D8A2B2490A3DAD8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F2740E1-C00E-4D77-B1C6-05E00C7F3DB0}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_5A6478FDB3C6AE02BECA10EA8A5A6CEF0C1AB86B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1D884FF-D2A4-4CDE-96D6-E0FE66B6A5E9}"/>
   <bookViews>
-    <workbookView xWindow="1995" yWindow="450" windowWidth="25185" windowHeight="14430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="1080" windowWidth="26415" windowHeight="14520" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comb Depth" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="vR Sort" sheetId="4" r:id="rId4"/>
     <sheet name="vL Depth" sheetId="5" r:id="rId5"/>
     <sheet name="vL Sort" sheetId="6" r:id="rId6"/>
+    <sheet name="Pot Depth" sheetId="7" r:id="rId7"/>
+    <sheet name="Pot Sort" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="68">
   <si>
     <t>Pos</t>
   </si>
@@ -41,139 +43,199 @@
     <t>C</t>
   </si>
   <si>
-    <t>Ian Leger</t>
+    <t>Yasmani Grandal</t>
   </si>
   <si>
     <t>1B</t>
   </si>
   <si>
-    <t>Omar Barragan</t>
-  </si>
-  <si>
-    <t>Nick Clements</t>
+    <t>Jose Ramirez</t>
   </si>
   <si>
     <t>2B</t>
   </si>
   <si>
-    <t>Billy Brenner</t>
+    <t>Francisco Lindor</t>
   </si>
   <si>
     <t>3B</t>
   </si>
   <si>
-    <t>Matt Mayes</t>
+    <t>Fernando Tatis Jr.</t>
   </si>
   <si>
     <t>SS</t>
   </si>
   <si>
-    <t>Ricky Estevez</t>
+    <t>Nolan Arenado</t>
   </si>
   <si>
     <t>LF</t>
   </si>
   <si>
+    <t>Mike Trout</t>
+  </si>
+  <si>
+    <t>Ronald Acuna Jr.</t>
+  </si>
+  <si>
+    <t>Juan Soto</t>
+  </si>
+  <si>
     <t>CF</t>
   </si>
   <si>
-    <t>Jesse Harwood</t>
-  </si>
-  <si>
-    <t>Johnny Dorn</t>
-  </si>
-  <si>
     <t>RF</t>
   </si>
   <si>
     <t>DH</t>
   </si>
   <si>
-    <t>Jason Palosaari</t>
+    <t>Vladimir Guerrero Jr.</t>
   </si>
   <si>
     <t>Names</t>
   </si>
   <si>
-    <t>Brian Flores</t>
-  </si>
-  <si>
-    <t>Don Tessier</t>
-  </si>
-  <si>
-    <t>Grant Stomski</t>
-  </si>
-  <si>
-    <t>Sean Cullinan</t>
-  </si>
-  <si>
-    <t>Dennis Green</t>
-  </si>
-  <si>
-    <t>Andy Wharton</t>
-  </si>
-  <si>
-    <t>Rich Ginzburg</t>
-  </si>
-  <si>
-    <t>Drew Condon</t>
-  </si>
-  <si>
-    <t>Alex McKinney</t>
-  </si>
-  <si>
-    <t>Joe MacIntyre</t>
-  </si>
-  <si>
-    <t>Mario Esquivel</t>
-  </si>
-  <si>
-    <t>John Rice</t>
-  </si>
-  <si>
-    <t>Allen Caravello</t>
-  </si>
-  <si>
-    <t>Kyle McGuire</t>
-  </si>
-  <si>
-    <t>Jeremy Hagerty</t>
-  </si>
-  <si>
-    <t>Franklin Lahoda</t>
-  </si>
-  <si>
-    <t>John Mann</t>
-  </si>
-  <si>
-    <t>Vinny Cordova</t>
-  </si>
-  <si>
-    <t>Dustin Johnston</t>
-  </si>
-  <si>
-    <t>Brian Hutt</t>
-  </si>
-  <si>
-    <t>Aaron Gomez</t>
-  </si>
-  <si>
-    <t>Jason Neely</t>
-  </si>
-  <si>
-    <t>Kenny Brawner</t>
-  </si>
-  <si>
-    <t>Carlos Carrillo</t>
-  </si>
-  <si>
-    <t>Matt Stankiewicz</t>
-  </si>
-  <si>
-    <t>Joe Bigelow</t>
-  </si>
-  <si>
-    <t>Donovan Johnson</t>
+    <t>Will Smith</t>
+  </si>
+  <si>
+    <t>J.T. Realmuto</t>
+  </si>
+  <si>
+    <t>Adley Rutschman</t>
+  </si>
+  <si>
+    <t>Carlos Correa</t>
+  </si>
+  <si>
+    <t>Keibert Ruiz</t>
+  </si>
+  <si>
+    <t>Trea Turner</t>
+  </si>
+  <si>
+    <t>Salvador Perez</t>
+  </si>
+  <si>
+    <t>Mookie Betts</t>
+  </si>
+  <si>
+    <t>Matt Chapman</t>
+  </si>
+  <si>
+    <t>Bryce Harper</t>
+  </si>
+  <si>
+    <t>Sean Murphy</t>
+  </si>
+  <si>
+    <t>Bo Bichette</t>
+  </si>
+  <si>
+    <t>Wander Franco</t>
+  </si>
+  <si>
+    <t>Brandon Crawford</t>
+  </si>
+  <si>
+    <t>Kyle Tucker</t>
+  </si>
+  <si>
+    <t>Cedric Mullins</t>
+  </si>
+  <si>
+    <t>Corey Seager</t>
+  </si>
+  <si>
+    <t>Byron Buxton</t>
+  </si>
+  <si>
+    <t>Harrison Bader</t>
+  </si>
+  <si>
+    <t>Shohei Ohtani</t>
+  </si>
+  <si>
+    <t>Joey Gallo</t>
+  </si>
+  <si>
+    <t>MJ Melendez</t>
+  </si>
+  <si>
+    <t>Xander Bogaerts</t>
+  </si>
+  <si>
+    <t>George Springer</t>
+  </si>
+  <si>
+    <t>Alex Bregman</t>
+  </si>
+  <si>
+    <t>Christian Vazquez</t>
+  </si>
+  <si>
+    <t>Mike Zunino</t>
+  </si>
+  <si>
+    <t>Wilmer Flores</t>
+  </si>
+  <si>
+    <t>Anthony Rendon</t>
+  </si>
+  <si>
+    <t>Tommy Edman</t>
+  </si>
+  <si>
+    <t>Luis Robert</t>
+  </si>
+  <si>
+    <t>Tim Anderson</t>
+  </si>
+  <si>
+    <t>Jose Trevino</t>
+  </si>
+  <si>
+    <t>Ozzie Albies</t>
+  </si>
+  <si>
+    <t>Stephen Vogt</t>
+  </si>
+  <si>
+    <t>Michael Brantley</t>
+  </si>
+  <si>
+    <t>Yordan Alvarez</t>
+  </si>
+  <si>
+    <t>Luis Garcia</t>
+  </si>
+  <si>
+    <t>Marcus Semien</t>
+  </si>
+  <si>
+    <t>Isiah Kiner-Falefa</t>
+  </si>
+  <si>
+    <t>Roberto Perez</t>
+  </si>
+  <si>
+    <t>Nicky Lopez</t>
+  </si>
+  <si>
+    <t>Austin Hedges</t>
+  </si>
+  <si>
+    <t>Ke'Bryan Hayes</t>
+  </si>
+  <si>
+    <t>Bryan Reynolds</t>
+  </si>
+  <si>
+    <t>Nick Ahmed</t>
+  </si>
+  <si>
+    <t>Bobby Witt Jr.</t>
   </si>
 </sst>
 </file>
@@ -493,13 +555,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -510,19 +573,19 @@
         <v>1</v>
       </c>
       <c r="C1">
-        <v>0.876956812188187</v>
+        <v>39.226047988073901</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1">
-        <v>0.87314299929035299</v>
+        <v>39.213146617059003</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
       </c>
       <c r="G1">
-        <v>0.84002587582518295</v>
+        <v>39.205561799642197</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -533,19 +596,19 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>-1.43127562204304</v>
+        <v>0.18088802191980799</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="E2">
-        <v>-1.43127562204304</v>
+        <v>0.18088802191980799</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
       </c>
       <c r="G2">
-        <v>-1.43127562204304</v>
+        <v>0.18088802191980799</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -556,134 +619,134 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>0.46204759325883299</v>
+        <v>5.7955201568916603</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
       <c r="E3">
-        <v>0.46204759325883299</v>
+        <v>5.7955201568916603</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G3">
-        <v>0.64642039436578003</v>
+        <v>5.7955201568916603</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4">
-        <v>0.37626534031820902</v>
+        <v>6.6567048011466898</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4">
-        <v>0.37626534031820902</v>
+        <v>6.6567048011466898</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="G4">
-        <v>0.37626534031820902</v>
+        <v>4.0108103904994099</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C5">
-        <v>0.34382364929958598</v>
+        <v>4.1308183945602899</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E5">
-        <v>0.34382364929958598</v>
+        <v>4.1308183945602899</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5">
-        <v>0.34382364929958598</v>
+        <v>6.7562266167759102</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>1.0023256948377099</v>
+        <v>4.6875186188526703</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E6">
-        <v>1.0023256948377099</v>
+        <v>4.6875186188526703</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G6">
-        <v>1.0023256948377099</v>
+        <v>4.6875186188526703</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C7">
-        <v>0.13579867284866901</v>
+        <v>5.5479487334026496</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E7">
-        <v>0.13579867284866901</v>
+        <v>4.1030413453646704</v>
       </c>
       <c r="F7" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G7">
-        <v>-8.5505064621281601E-2</v>
+        <v>5.5479487334026496</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8">
-        <v>-0.53978609104416198</v>
+        <v>3.4590954536566501</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E8">
-        <v>-0.308745065240217</v>
+        <v>3.4590954536566501</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G8">
-        <v>-0.53978609104416198</v>
+        <v>3.4590954536566501</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -691,22 +754,22 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9">
-        <v>9.2111211142592603E-2</v>
+        <v>3.8025985170144199</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
       </c>
       <c r="E9">
-        <v>-0.14274362755918599</v>
+        <v>5.2346045340375102</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G9">
-        <v>9.2111211142592603E-2</v>
+        <v>3.8025985170144199</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -717,19 +780,19 @@
         <v>19</v>
       </c>
       <c r="C10">
-        <v>0.43564636356978897</v>
+        <v>4.9649552906290602</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
       </c>
       <c r="E10">
-        <v>0.43564636356978897</v>
+        <v>4.9649552906290602</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
       </c>
       <c r="G10">
-        <v>0.43564636356978897</v>
+        <v>4.9649552906290602</v>
       </c>
     </row>
   </sheetData>
@@ -741,7 +804,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O6" sqref="O6:P6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -762,31 +827,31 @@
         <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
         <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" t="s">
         <v>20</v>
       </c>
       <c r="J1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K1" t="s">
         <v>20</v>
       </c>
       <c r="L1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M1" t="s">
         <v>20</v>
       </c>
       <c r="N1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="O1" t="s">
         <v>20</v>
@@ -803,506 +868,506 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>-1.2096486697536999</v>
+        <v>0.18088802191980799</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2">
-        <v>1.0198732885800801</v>
+        <v>7.0379099008431698</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F2">
-        <v>1.12841169458952</v>
+        <v>6.6567048011466898</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2">
-        <v>0.34382364929958598</v>
+        <v>6.7562266167759102</v>
       </c>
       <c r="I2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="J2">
-        <v>1.0023256948377099</v>
+        <v>6.18200559218851</v>
       </c>
       <c r="K2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="L2">
-        <v>0.13579867284866901</v>
+        <v>5.5479487334026496</v>
       </c>
       <c r="M2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="N2">
-        <v>-0.308745065240217</v>
+        <v>3.4590954536566501</v>
       </c>
       <c r="O2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P2">
-        <v>9.2111211142592603E-2</v>
+        <v>5.2346045340375102</v>
       </c>
       <c r="Q2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="R2">
-        <v>0.76570579816870399</v>
+        <v>5.5603941135095001</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B3">
-        <v>-1.3846144948421799</v>
+        <v>-0.23424088728741599</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>0.64642039436578003</v>
+        <v>5.7955201568916603</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>0.37626534031820902</v>
+        <v>4.7748930588672902</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H3">
-        <v>-0.379058152095894</v>
+        <v>4.4664207540645098</v>
       </c>
       <c r="I3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J3">
-        <v>-0.26557716862595199</v>
+        <v>4.6875186188526703</v>
       </c>
       <c r="K3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="L3">
-        <v>7.0223263477275394E-2</v>
+        <v>5.1556379100286298</v>
       </c>
       <c r="M3" t="s">
         <v>15</v>
       </c>
       <c r="N3">
-        <v>-0.53978609104416198</v>
+        <v>3.4178024440568202</v>
       </c>
       <c r="O3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="P3">
-        <v>-3.9161853506848601E-2</v>
+        <v>4.8033873312794704</v>
       </c>
       <c r="Q3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="R3">
-        <v>0.43564636356978897</v>
+        <v>5.1913361437482202</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B4">
-        <v>-1.43127562204304</v>
+        <v>-0.57887825366409196</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>0.46204759325883299</v>
+        <v>5.0105817521287603</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="F4">
-        <v>-0.153107450839811</v>
+        <v>4.1512946600387899</v>
       </c>
       <c r="G4" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="H4">
-        <v>-0.43794554580287298</v>
+        <v>4.1308183945602899</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J4">
-        <v>-1.2944964638893699</v>
+        <v>4.3117106922584698</v>
       </c>
       <c r="K4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="L4">
-        <v>-8.5505064621281601E-2</v>
+        <v>5.0617060608859097</v>
       </c>
       <c r="M4" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="N4">
-        <v>-1.0217058067020699</v>
+        <v>3.12124372149303</v>
       </c>
       <c r="O4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4">
+        <v>4.7989814142487903</v>
+      </c>
+      <c r="Q4" t="s">
         <v>19</v>
       </c>
-      <c r="P4">
-        <v>-0.108553257832378</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>6</v>
-      </c>
       <c r="R4">
-        <v>0.40099684277806402</v>
+        <v>4.9649552906290602</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B5">
-        <v>-1.5743576251443401</v>
+        <v>-0.80924945774100099</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="D5">
-        <v>0.219227614821313</v>
+        <v>4.4151429292483204</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F5">
-        <v>-0.54211985261540296</v>
+        <v>4.0108103904994099</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H5">
-        <v>-0.516349429929151</v>
+        <v>4.0311581844196702</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="J5">
-        <v>-1.6154002798012801</v>
+        <v>4.2207680363984901</v>
       </c>
       <c r="K5" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="L5">
-        <v>-0.124116087994532</v>
+        <v>4.1169022602215097</v>
       </c>
       <c r="M5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="N5">
-        <v>-1.14680010234875</v>
+        <v>2.38919533073003</v>
       </c>
       <c r="O5" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="P5">
-        <v>-0.14274362755918599</v>
+        <v>3.8129511066469202</v>
       </c>
       <c r="Q5" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="R5">
-        <v>4.0385731929767001E-2</v>
+        <v>4.3637170458392802</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>-1.2144406483710199</v>
+      </c>
+      <c r="C6" t="s">
         <v>26</v>
       </c>
-      <c r="B6">
-        <v>-1.7055827087222399</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
       <c r="D6">
-        <v>0.17202091742574299</v>
+        <v>4.3234750952754704</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F6">
-        <v>-0.69230742332524398</v>
+        <v>4.0099835265868604</v>
       </c>
       <c r="G6" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="H6">
-        <v>-0.62748675890725403</v>
+        <v>3.2668874228243499</v>
       </c>
       <c r="I6" t="s">
         <v>5</v>
       </c>
       <c r="J6">
-        <v>-1.7275961576199499</v>
+        <v>3.3445023879710498</v>
       </c>
       <c r="K6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L6">
-        <v>-0.18392665546533801</v>
+        <v>4.1030413453646704</v>
       </c>
       <c r="M6" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="N6">
-        <v>-1.18824736292424</v>
+        <v>2.1262978152060801</v>
       </c>
       <c r="O6" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="P6">
-        <v>-0.19284224807015701</v>
+        <v>3.8025985170144199</v>
       </c>
       <c r="Q6" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="R6">
-        <v>-5.3268573401180101E-3</v>
+        <v>3.6803212044832101</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B7">
-        <v>-2.0606376094703598</v>
+        <v>-1.28188217246777</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D7">
-        <v>0.14475116932999799</v>
+        <v>4.2268411310064504</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F7">
-        <v>-0.78452188929810696</v>
+        <v>3.2062140329820701</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="H7">
-        <v>-0.68808914431655399</v>
+        <v>3.14747775259297</v>
       </c>
       <c r="I7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J7">
-        <v>-1.9335098656820999</v>
+        <v>2.5838839809905698</v>
       </c>
       <c r="K7" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="L7">
-        <v>-0.25688779939953799</v>
+        <v>3.5468668299451398</v>
       </c>
       <c r="M7" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="N7">
-        <v>-1.2765086570720201</v>
+        <v>1.99032654576232</v>
       </c>
       <c r="O7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="P7">
-        <v>-0.244024205444628</v>
+        <v>3.3091545367631898</v>
       </c>
       <c r="Q7" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="R7">
-        <v>-0.171783296633048</v>
+        <v>3.64075452666463</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B8">
-        <v>-2.10635019874025</v>
+        <v>-1.29838822681718</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D8">
-        <v>-0.24835462741116601</v>
+        <v>3.98302191365253</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="F8">
-        <v>-0.96743371594907601</v>
+        <v>3.1968006874838499</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="H8">
-        <v>-0.90364947713569399</v>
+        <v>3.12926505653029</v>
       </c>
       <c r="I8" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="J8">
-        <v>-2.2635988674324601</v>
+        <v>2.5104259316075099</v>
       </c>
       <c r="K8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="L8">
-        <v>-0.37132328617327798</v>
+        <v>3.5423658498068198</v>
       </c>
       <c r="M8" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="N8">
-        <v>-1.3125200500954699</v>
+        <v>1.8998994180683699</v>
       </c>
       <c r="O8" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="P8">
-        <v>-0.28255356766817202</v>
+        <v>3.2417274786996302</v>
       </c>
       <c r="Q8" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="R8">
-        <v>-0.25352111562512603</v>
+        <v>3.5861917492470101</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="B9">
-        <v>-2.1471377645554601</v>
+        <v>-1.30714669470789</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9">
-        <v>-0.25764290663327699</v>
+        <v>3.8831187218605501</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="F9">
-        <v>-1.19466383804841</v>
+        <v>3.0684421253954102</v>
       </c>
       <c r="G9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H9">
-        <v>-1.37654796534271</v>
+        <v>2.8977417281792901</v>
       </c>
       <c r="I9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9">
+        <v>1.8181434057199799</v>
+      </c>
+      <c r="K9" t="s">
         <v>32</v>
       </c>
-      <c r="J9">
-        <v>-2.62426294211012</v>
-      </c>
-      <c r="K9" t="s">
-        <v>15</v>
-      </c>
       <c r="L9">
-        <v>-0.387831818929399</v>
+        <v>3.3118876160717199</v>
       </c>
       <c r="M9" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="N9">
-        <v>-1.34795547905207</v>
+        <v>1.76324989314531</v>
       </c>
       <c r="O9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="P9">
-        <v>-0.58266507519275201</v>
+        <v>3.0558853203084899</v>
       </c>
       <c r="Q9" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="R9">
-        <v>-0.40053954013278698</v>
+        <v>3.5054339547032001</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B10">
-        <v>-2.2288755835475298</v>
+        <v>-1.3709087690963899</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D10">
-        <v>-0.40010259646397001</v>
+        <v>3.8586408016352598</v>
       </c>
       <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10">
+        <v>2.8003438636264502</v>
+      </c>
+      <c r="G10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10">
+        <v>2.71342198189482</v>
+      </c>
+      <c r="I10" t="s">
         <v>32</v>
       </c>
-      <c r="F10">
-        <v>-1.20357850786795</v>
-      </c>
-      <c r="G10" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10">
-        <v>-1.4643679170833399</v>
-      </c>
-      <c r="I10" t="s">
-        <v>6</v>
-      </c>
       <c r="J10">
-        <v>-2.66866653014598</v>
+        <v>1.7758233620858299</v>
       </c>
       <c r="K10" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="L10">
-        <v>-0.57236038397109601</v>
+        <v>3.3077427536161599</v>
       </c>
       <c r="M10" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="N10">
-        <v>-1.4347335509492101</v>
+        <v>1.7273673738798001</v>
       </c>
       <c r="O10" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="P10">
-        <v>-0.62514004459550399</v>
+        <v>2.9884832728051101</v>
       </c>
       <c r="Q10" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="R10">
-        <v>-0.61057541260918202</v>
+        <v>3.4252785348915502</v>
       </c>
     </row>
   </sheetData>
@@ -1314,7 +1379,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1326,19 +1393,19 @@
         <v>1</v>
       </c>
       <c r="C1">
-        <v>3.6354234102197598</v>
+        <v>38.607172869764298</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1">
-        <v>3.6316095973219298</v>
+        <v>38.586686681332701</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
       </c>
       <c r="G1">
-        <v>3.5347270602146601</v>
+        <v>38.586558859546102</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1346,22 +1413,22 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>-0.826024290924391</v>
+        <v>0.37798749437110302</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>-0.826024290924391</v>
+        <v>0.37798749437110302</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="G2">
-        <v>-0.826024290924391</v>
+        <v>0.37798749437110302</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1372,134 +1439,134 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>1.0329625344553901</v>
+        <v>5.6818769011342303</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
       <c r="E3">
-        <v>1.0329625344553901</v>
+        <v>5.6818769011342303</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
       </c>
       <c r="G3">
-        <v>1.0329625344553901</v>
+        <v>5.6818769011342303</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C4">
-        <v>0.24822213373708699</v>
+        <v>3.5682424208493599</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4">
-        <v>0.24822213373708699</v>
+        <v>6.4282008021145201</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="G4">
-        <v>0.24822213373708699</v>
+        <v>3.5682424208493599</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>0.161082799238979</v>
+        <v>6.5277226177437404</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="E5">
-        <v>0.161082799238979</v>
+        <v>3.6472780480469198</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5">
-        <v>0.161082799238979</v>
+        <v>6.5277226177437404</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>1.4136736597209301</v>
+        <v>4.7864766204617597</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E6">
-        <v>1.4136736597209301</v>
+        <v>4.7864766204617597</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G6">
-        <v>1.4136736597209301</v>
+        <v>4.7864766204617597</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
       <c r="C7">
-        <v>0.20901919109550601</v>
+        <v>5.1553659526659903</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E7">
-        <v>0.20901919109550601</v>
+        <v>5.1553659526659903</v>
       </c>
       <c r="F7" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G7">
-        <v>0.66421623376212602</v>
+        <v>5.9169094687570398</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="C8">
-        <v>-0.103260399279101</v>
+        <v>2.2164228437593199</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="E8">
-        <v>0.16947710210102801</v>
+        <v>2.2164228437593199</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G8">
-        <v>-0.103260399279101</v>
+        <v>3.4588234962940101</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1507,22 +1574,22 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9">
-        <v>0.57033337848383703</v>
+        <v>5.6035652693918996</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
       </c>
       <c r="E9">
-        <v>0.29378206420587399</v>
+        <v>5.6035652693918996</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="G9">
-        <v>0.57033337848383703</v>
+        <v>3.5790070905479299</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1530,22 +1597,22 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C10">
-        <v>0.92941440369152195</v>
+        <v>4.68951274938693</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E10">
-        <v>0.92941440369152195</v>
+        <v>4.68951274938693</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G10">
-        <v>0.373521011019805</v>
+        <v>4.68951274938693</v>
       </c>
     </row>
   </sheetData>
@@ -1578,31 +1645,31 @@
         <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
         <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" t="s">
         <v>20</v>
       </c>
       <c r="J1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K1" t="s">
         <v>20</v>
       </c>
       <c r="L1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M1" t="s">
         <v>20</v>
       </c>
       <c r="N1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="O1" t="s">
         <v>20</v>
@@ -1619,506 +1686,506 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>-0.826024290924391</v>
+        <v>0.37798749437110302</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2">
-        <v>1.1748379552792401</v>
+        <v>6.8094059018110098</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F2">
-        <v>1.5397596594727401</v>
+        <v>6.4282008021145201</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2">
-        <v>0.161082799238979</v>
+        <v>6.5277226177437404</v>
       </c>
       <c r="I2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="J2">
-        <v>1.4136736597209301</v>
+        <v>5.9535015931563402</v>
       </c>
       <c r="K2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="L2">
-        <v>0.66421623376212602</v>
+        <v>5.9169094687570398</v>
       </c>
       <c r="M2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N2">
-        <v>0.16947710210102801</v>
+        <v>3.78676317941121</v>
       </c>
       <c r="O2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P2">
-        <v>0.57033337848383703</v>
+        <v>5.6035652693918996</v>
       </c>
       <c r="Q2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="R2">
-        <v>0.99423656748758105</v>
+        <v>5.9293548488638903</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B3">
-        <v>-1.04594006423089</v>
+        <v>-0.54863750160082203</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3">
-        <v>1.0329625344553901</v>
+        <v>5.6818769011342303</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>0.24822213373708699</v>
+        <v>4.6612498031098601</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H3">
-        <v>9.0472015110583906E-2</v>
+        <v>4.3527774983070797</v>
       </c>
       <c r="I3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J3">
-        <v>-0.39362037520707399</v>
+        <v>4.7864766204617597</v>
       </c>
       <c r="K3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="L3">
-        <v>0.62881346739506805</v>
+        <v>5.1553659526659903</v>
       </c>
       <c r="M3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="N3">
-        <v>-0.103260399279101</v>
+        <v>3.4588234962940101</v>
       </c>
       <c r="O3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="P3">
-        <v>0.48925570740660901</v>
+        <v>4.80311537391683</v>
       </c>
       <c r="Q3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="R3">
-        <v>0.92941440369152195</v>
+        <v>4.9628321447160602</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B4">
-        <v>-1.3923895198143099</v>
+        <v>-0.62967847479324301</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>0.83713243851947505</v>
+        <v>5.3795424874831497</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F4">
-        <v>2.8795088581158101E-2</v>
+        <v>4.2502526616478802</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="H4">
-        <v>3.2289812787326601E-2</v>
+        <v>3.6472780480469198</v>
       </c>
       <c r="I4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="J4">
-        <v>-1.1566812164233899</v>
+        <v>3.80463250665907</v>
       </c>
       <c r="K4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="L4">
-        <v>0.48540987657528001</v>
+        <v>4.8332020618537497</v>
       </c>
       <c r="M4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N4">
-        <v>-0.74809109615856295</v>
+        <v>2.8927397224608602</v>
       </c>
       <c r="O4" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="P4">
-        <v>0.450036946085414</v>
+        <v>4.5704774152166197</v>
       </c>
       <c r="Q4" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="R4">
-        <v>0.58296494810809696</v>
+        <v>4.68951274938693</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="B5">
-        <v>-1.53543525754368</v>
+        <v>-0.70245270536047899</v>
       </c>
       <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5">
+        <v>4.48282220910649</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5">
+        <v>3.5682424208493599</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5">
+        <v>3.6237402089608799</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5">
+        <v>3.6807788543411499</v>
+      </c>
+      <c r="K5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <v>4.0032590044640797</v>
+      </c>
+      <c r="M5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N5">
+        <v>2.2164228437593199</v>
+      </c>
+      <c r="O5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P5">
+        <v>3.6993078508894799</v>
+      </c>
+      <c r="Q5" t="s">
         <v>19</v>
       </c>
-      <c r="D5">
-        <v>0.77781781873910605</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5">
-        <v>-0.15985789602662201</v>
-      </c>
-      <c r="G5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5">
-        <v>-5.6571817710692897E-2</v>
-      </c>
-      <c r="I5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5">
-        <v>-1.4482431875170101</v>
-      </c>
-      <c r="K5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5">
-        <v>0.29429551187590602</v>
-      </c>
-      <c r="M5" t="s">
-        <v>19</v>
-      </c>
-      <c r="N5">
-        <v>-0.78936527513428201</v>
-      </c>
-      <c r="O5" t="s">
-        <v>5</v>
-      </c>
-      <c r="P5">
-        <v>0.37807269312640401</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>5</v>
-      </c>
       <c r="R5">
-        <v>0.56558808385644399</v>
+        <v>4.6284853245346298</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B6">
-        <v>-1.6462638850165701</v>
+        <v>-0.91140776844469795</v>
       </c>
       <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>4.0786729631538998</v>
+      </c>
+      <c r="E6" t="s">
         <v>24</v>
       </c>
-      <c r="D6">
-        <v>0.47788644842003603</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
       <c r="F6">
-        <v>-0.43901615503561903</v>
+        <v>3.5037322049000101</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H6">
-        <v>-0.64439263651027401</v>
+        <v>3.4911690023623301</v>
       </c>
       <c r="I6" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="J6">
-        <v>-1.62215072498809</v>
+        <v>3.2308591322136202</v>
       </c>
       <c r="K6" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="L6">
-        <v>0.20901919109550601</v>
+        <v>3.8841464417934399</v>
       </c>
       <c r="M6" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="N6">
-        <v>-0.86381860975264801</v>
+        <v>2.1216142827179798</v>
       </c>
       <c r="O6" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="P6">
-        <v>0.29378206420587399</v>
+        <v>3.5790070905479299</v>
       </c>
       <c r="Q6" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="R6">
-        <v>0.373521011019805</v>
+        <v>4.2500737900818502</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7">
-        <v>-1.7275023303803201</v>
+        <v>-0.97647106540276896</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D7">
-        <v>0.15370505824994299</v>
+        <v>4.0474626302264598</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="F7">
-        <v>-0.55910508348607002</v>
+        <v>3.4699943445295198</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="H7">
-        <v>-0.783425225684797</v>
+        <v>3.4425948549395202</v>
       </c>
       <c r="I7" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J7">
-        <v>-1.7080930598700701</v>
+        <v>3.1521012521979199</v>
       </c>
       <c r="K7" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="L7">
-        <v>4.8693872835661602E-2</v>
+        <v>3.7962182847891999</v>
       </c>
       <c r="M7" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="N7">
-        <v>-0.97938477100543297</v>
+        <v>2.1005295049936099</v>
       </c>
       <c r="O7" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="P7">
-        <v>8.9111073645409794E-2</v>
+        <v>3.5759083427604499</v>
       </c>
       <c r="Q7" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="R7">
-        <v>-0.18197658654115201</v>
+        <v>4.2346068277478999</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B8">
-        <v>-1.8269446985800499</v>
+        <v>-1.28193369220297</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D8">
-        <v>7.66848360575004E-2</v>
+        <v>4.0227279169583703</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F8">
-        <v>-0.84605414695288705</v>
+        <v>3.3015006448279101</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="H8">
-        <v>-0.910399922322504</v>
+        <v>3.3434995459680201</v>
       </c>
       <c r="I8" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="J8">
-        <v>-2.1402489692325202</v>
+        <v>2.3377809342375402</v>
       </c>
       <c r="K8" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="L8">
-        <v>-0.43962864946014502</v>
+        <v>3.75039931671233</v>
       </c>
       <c r="M8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N8">
-        <v>-1.0489424923105699</v>
+        <v>2.0194384290829799</v>
       </c>
       <c r="O8" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="P8">
-        <v>-0.46719977349749398</v>
+        <v>3.5188410331111899</v>
       </c>
       <c r="Q8" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="R8">
-        <v>-0.26711937800129099</v>
+        <v>3.6404825693020002</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B9">
-        <v>-2.1303733578832098</v>
+        <v>-1.5075443954363801</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D9">
-        <v>-0.246871327391089</v>
+        <v>4.0101584733450304</v>
       </c>
       <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9">
+        <v>3.0021008189340002</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>3.22822305813939</v>
+      </c>
+      <c r="I9" t="s">
         <v>37</v>
       </c>
-      <c r="F9">
-        <v>-1.3021442965007699</v>
-      </c>
-      <c r="G9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9">
-        <v>-1.0555797617041001</v>
-      </c>
-      <c r="I9" t="s">
-        <v>29</v>
-      </c>
       <c r="J9">
-        <v>-2.33597128610569</v>
+        <v>2.3179437011739301</v>
       </c>
       <c r="K9" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="L9">
-        <v>-0.48185732387410302</v>
+        <v>3.73328444371761</v>
       </c>
       <c r="M9" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="N9">
-        <v>-1.26225274215087</v>
+        <v>2.01265455944865</v>
       </c>
       <c r="O9" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="P9">
-        <v>-0.52310050311697498</v>
+        <v>3.4328416153673702</v>
       </c>
       <c r="Q9" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="R9">
-        <v>-0.52420343539611003</v>
+        <v>3.5031586026746901</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B10">
-        <v>-2.23201183349344</v>
+        <v>-1.66562765562649</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D10">
-        <v>-0.25510507259797599</v>
+        <v>3.8828503135248398</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F10">
-        <v>-1.3053817996378101</v>
+        <v>2.8834840655534002</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H10">
-        <v>-1.2693226162648601</v>
+        <v>2.8859425553631999</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="J10">
-        <v>-2.5526541330871</v>
+        <v>1.8067492183155001</v>
       </c>
       <c r="K10" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="L10">
-        <v>-0.61187022162208204</v>
+        <v>3.5217694921665101</v>
       </c>
       <c r="M10" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="N10">
-        <v>-1.2895373669374399</v>
+        <v>1.92120419628741</v>
       </c>
       <c r="O10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P10">
-        <v>-0.71871720070505696</v>
+        <v>3.1364972545995</v>
       </c>
       <c r="Q10" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="R10">
-        <v>-0.56118577933853198</v>
+        <v>3.4886135644651799</v>
       </c>
     </row>
   </sheetData>
@@ -2130,9 +2197,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2142,19 +2214,19 @@
         <v>1</v>
       </c>
       <c r="C1">
-        <v>2.7837307491775198</v>
+        <v>44.935165404998997</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1">
-        <v>2.7758061009706299</v>
+        <v>44.883357654600097</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
       </c>
       <c r="G1">
-        <v>2.7440772807974798</v>
+        <v>44.865535801483198</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2162,22 +2234,22 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C2">
-        <v>-0.53776311518100195</v>
+        <v>1.3124149487801</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E2">
-        <v>-0.53776311518100195</v>
+        <v>1.3124149487801</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="G2">
-        <v>-0.53776311518100195</v>
+        <v>1.3124149487801</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2185,137 +2257,137 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>0.56824711079812296</v>
+        <v>6.0965239007637804</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>0.56824711079812296</v>
+        <v>6.0965239007637804</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="G3">
-        <v>0.56824711079812296</v>
+        <v>6.0965239007637804</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>0.90842558440111298</v>
+        <v>5.4402379166638104</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E4">
-        <v>0.90842558440111298</v>
+        <v>5.4402379166638104</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="G4">
-        <v>-5.3320817497022298E-2</v>
+        <v>7.2619370143564597</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>1.10331271528575</v>
+        <v>7.36145882998568</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5">
-        <v>1.10331271528575</v>
+        <v>7.36145882998568</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="G5">
-        <v>1.10331271528575</v>
+        <v>5.4739023398768003</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>5.6547946375749802</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6">
+        <v>5.6547946375749802</v>
+      </c>
+      <c r="F6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6">
-        <v>-0.65550985806114404</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6">
-        <v>-0.65550985806114404</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
       <c r="G6">
-        <v>0.26658307545695198</v>
+        <v>5.6510224264754498</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
       <c r="C7">
-        <v>0.62841359405494801</v>
+        <v>5.1563582359624496</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E7">
-        <v>0.62841359405494801</v>
+        <v>5.08240620935522</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="G7">
-        <v>0.62841359405494801</v>
+        <v>5.1563582359624496</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C8">
-        <v>-0.55356989833069703</v>
+        <v>3.2752595838715499</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E8">
-        <v>-0.275048747735824</v>
+        <v>3.2752595838715499</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="G8">
-        <v>-0.55356989833069703</v>
+        <v>3.2752595838715499</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2323,22 +2395,22 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="C9">
-        <v>0.297010927627055</v>
+        <v>4.78196338100497</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E9">
-        <v>1.0565128825298999E-2</v>
+        <v>4.8041076572132901</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="G9">
-        <v>0.297010927627055</v>
+        <v>4.78196338100497</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2346,22 +2418,22 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C10">
-        <v>1.0251636885833699</v>
+        <v>5.8561539703916798</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E10">
-        <v>1.0251636885833699</v>
+        <v>5.8561539703916798</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="G10">
-        <v>1.0251636885833699</v>
+        <v>5.8561539703916798</v>
       </c>
     </row>
   </sheetData>
@@ -2394,31 +2466,31 @@
         <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
         <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" t="s">
         <v>20</v>
       </c>
       <c r="J1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K1" t="s">
         <v>20</v>
       </c>
       <c r="L1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M1" t="s">
         <v>20</v>
       </c>
       <c r="N1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="O1" t="s">
         <v>20</v>
@@ -2435,450 +2507,1271 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B2">
-        <v>-0.45015960376754099</v>
+        <v>1.3124149487801</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2">
-        <v>1.77936235456624</v>
+        <v>7.6431421140529396</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2">
-        <v>0.90842558440111298</v>
+        <v>7.2619370143564597</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2">
-        <v>1.10331271528575</v>
+        <v>7.36145882998568</v>
       </c>
       <c r="I2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J2">
-        <v>0.26658307545695198</v>
+        <v>6.78723780539827</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="L2">
-        <v>0.62841359405494801</v>
+        <v>5.6669382740956804</v>
       </c>
       <c r="M2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="N2">
-        <v>-2.1968926473844401E-2</v>
+        <v>3.7264759347027998</v>
       </c>
       <c r="O2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="P2">
-        <v>0.71718331256005496</v>
+        <v>5.4042136274585504</v>
       </c>
       <c r="Q2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="R2">
-        <v>1.52519486415487</v>
+        <v>5.8561539703916798</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B3">
-        <v>-0.53776311518100195</v>
+        <v>0.59849271699307405</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>0.70784965048944504</v>
+        <v>6.0965239007637804</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F3">
-        <v>-5.3320817497022298E-2</v>
+        <v>5.4402379166638104</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H3">
-        <v>1.5810814153752399E-2</v>
+        <v>5.4739023398768003</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J3">
-        <v>-0.65550985806114404</v>
+        <v>5.6547946375749802</v>
       </c>
       <c r="K3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L3">
-        <v>0.50260126658662496</v>
+        <v>5.1563582359624496</v>
       </c>
       <c r="M3" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="N3">
-        <v>-0.275048747735824</v>
+        <v>3.45981577959048</v>
       </c>
       <c r="O3" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="P3">
-        <v>0.297010927627055</v>
+        <v>4.8041076572132901</v>
       </c>
       <c r="Q3" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="R3">
-        <v>1.0251636885833699</v>
+        <v>5.79656835695799</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B4">
-        <v>-0.95019077933903795</v>
+        <v>0.47421481439648799</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D4">
-        <v>0.56824711079812296</v>
+        <v>5.3133731119375103</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F4">
-        <v>-0.125051932283228</v>
+        <v>5.3538943358159203</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="H4">
-        <v>-0.29186295094417403</v>
+        <v>5.46141257449663</v>
       </c>
       <c r="I4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J4">
-        <v>-0.70727717469502505</v>
+        <v>5.6510224264754498</v>
       </c>
       <c r="K4" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="L4">
-        <v>0.118423130024672</v>
+        <v>5.08240620935522</v>
       </c>
       <c r="M4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="N4">
-        <v>-0.54926075709601596</v>
+        <v>3.3685601947205801</v>
       </c>
       <c r="O4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="P4">
-        <v>1.3846561232717301E-2</v>
+        <v>4.78196338100497</v>
       </c>
       <c r="Q4" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="R4">
-        <v>0.38916146761904502</v>
+        <v>4.6647207897114003</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B5">
-        <v>-1.2011902628473501</v>
+        <v>-0.325691323403831</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D5">
-        <v>0.52449316637125398</v>
+        <v>5.3063416090109401</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>-0.43517477206225003</v>
+        <v>5.0758968027394102</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="H5">
-        <v>-0.83915878022299395</v>
+        <v>4.7674244979366298</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="J5">
-        <v>-1.5873447612447</v>
+        <v>4.4254113008960196</v>
       </c>
       <c r="K5" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="L5">
-        <v>-0.13424879257531899</v>
+        <v>4.7821180902905702</v>
       </c>
       <c r="M5" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="N5">
-        <v>-0.55356989833069703</v>
+        <v>3.2752595838715499</v>
       </c>
       <c r="O5" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="P5">
-        <v>1.0565128825298999E-2</v>
+        <v>4.4804870642694201</v>
       </c>
       <c r="Q5" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="R5">
-        <v>0.22444289673933199</v>
+        <v>4.5831380331263896</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>-1.71186187378108</v>
+        <v>-0.34116389156720001</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="D6">
-        <v>0.13205764761893299</v>
+        <v>5.2073586041781201</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F6">
-        <v>-0.58119117494321904</v>
+        <v>4.0266737458528503</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="H6">
-        <v>-0.87559395857911104</v>
+        <v>4.4356469382597501</v>
       </c>
       <c r="I6" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="J6">
-        <v>-1.9628119298480899</v>
+        <v>3.6455061318431699</v>
       </c>
       <c r="K6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="L6">
-        <v>-0.14333154851728699</v>
+        <v>4.57069265301954</v>
       </c>
       <c r="M6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N6">
-        <v>-1.51673799080312</v>
+        <v>2.8104652485225601</v>
       </c>
       <c r="O6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="P6">
-        <v>-8.7806934202229597E-2</v>
+        <v>4.2573484536543997</v>
       </c>
       <c r="Q6" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="R6">
-        <v>0.11341985251862299</v>
+        <v>4.5655566132375602</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B7">
-        <v>-1.7509115711830801</v>
+        <v>-0.395267609830109</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D7">
-        <v>-0.16148237503218901</v>
+        <v>5.2017247469517702</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F7">
-        <v>-0.78047394774926204</v>
+        <v>3.8907562212654399</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="H7">
-        <v>-1.00281382805206</v>
+        <v>3.6397371123997302</v>
       </c>
       <c r="I7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J7">
-        <v>-2.2011583819914402</v>
+        <v>3.2357303044460899</v>
       </c>
       <c r="K7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="L7">
-        <v>-0.14470498344763699</v>
+        <v>4.4335645295694404</v>
       </c>
       <c r="M7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="N7">
-        <v>-1.8626172838372199</v>
+        <v>2.5592767104960399</v>
       </c>
       <c r="O7" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="P7">
-        <v>-0.468046476335091</v>
+        <v>4.2003532165258104</v>
       </c>
       <c r="Q7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="R7">
-        <v>-0.339091560281223</v>
+        <v>4.0980883813885702</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="B8">
-        <v>-1.87944891125465</v>
+        <v>-0.53866556972656499</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D8">
-        <v>-0.17041329734895</v>
+        <v>5.1533481536444796</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="F8">
-        <v>-0.90783977409062899</v>
+        <v>3.8891873420821401</v>
       </c>
       <c r="G8" t="s">
         <v>32</v>
       </c>
       <c r="H8">
-        <v>-1.08998284607563</v>
+        <v>3.4383707447694398</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="J8">
-        <v>-2.2313448258139101</v>
+        <v>2.5937264535981801</v>
       </c>
       <c r="K8" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="L8">
-        <v>-0.17613419059871599</v>
+        <v>4.4179060040936404</v>
       </c>
       <c r="M8" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="N8">
-        <v>-1.8666166130189199</v>
+        <v>2.4405463636737101</v>
       </c>
       <c r="O8" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="P8">
-        <v>-0.67969357081928605</v>
+        <v>4.1139548505190398</v>
       </c>
       <c r="Q8" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="R8">
-        <v>-0.37819772511226601</v>
+        <v>4.0424149706611301</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B9">
-        <v>-1.9876034888815</v>
+        <v>-0.77635885533629001</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D9">
-        <v>-0.18311113066610499</v>
+        <v>5.0291421504515901</v>
       </c>
       <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9">
+        <v>3.7468430495722198</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9">
+        <v>3.3306935090497301</v>
+      </c>
+      <c r="I9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9">
+        <v>2.41619112373581</v>
+      </c>
+      <c r="K9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9">
+        <v>4.1212099359542904</v>
+      </c>
+      <c r="M9" t="s">
+        <v>5</v>
+      </c>
+      <c r="N9">
+        <v>2.4273015590782001</v>
+      </c>
+      <c r="O9" t="s">
+        <v>26</v>
+      </c>
+      <c r="P9">
+        <v>3.8025021155829499</v>
+      </c>
+      <c r="Q9" t="s">
         <v>45</v>
       </c>
+      <c r="R9">
+        <v>4.0121096854417804</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10">
+        <v>-0.96397704058919098</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10">
+        <v>4.7674701475965904</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10">
+        <v>3.5811876736338202</v>
+      </c>
+      <c r="G10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10">
+        <v>3.3128216126101502</v>
+      </c>
+      <c r="I10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10">
+        <v>2.3164523786759799</v>
+      </c>
+      <c r="K10" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10">
+        <v>3.9127848877988201</v>
+      </c>
+      <c r="M10" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10">
+        <v>2.4171783295909801</v>
+      </c>
+      <c r="O10" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10">
+        <v>3.67302175607806</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>48</v>
+      </c>
+      <c r="R10">
+        <v>3.73423735929895</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.8" bottom="0.8" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>25.457262673858999</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>25.444361302844101</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1">
+        <v>25.351215364091701</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>1.4962550278987601</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2">
+        <v>1.4962550278987601</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2">
+        <v>1.4962550278987601</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>3.03604183141581</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3">
+        <v>3.03604183141581</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>3.87466033165438</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>2.8540332336300098</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>2.8540332336300098</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4">
+        <v>1.90936742362418</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>4.5103656646585701</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>4.5103656646585701</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <v>4.5103656646585701</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>3.4772892028063902</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>3.4772892028063902</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6">
+        <v>3.4772892028063902</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>2.8118528717782199</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>3.2218037518406799</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7">
+        <v>2.8118528717782199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8">
+        <v>1.44650071331367</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8">
+        <v>1.44650071331367</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8">
+        <v>1.44650071331367</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>2.9213609234904401</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>2.4985086724130898</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>2.9213609234904401</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>2.9035632048670901</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10">
+        <v>2.9035632048670901</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10">
+        <v>2.9035632048670901</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.8" bottom="0.8" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:R10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>1.4962550278987601</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>4.7920489487258298</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>4.4108438490293498</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <v>4.5103656646585701</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2">
+        <v>3.9361446400711602</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2">
+        <v>3.2218037518406799</v>
+      </c>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2">
+        <v>1.50795773720605</v>
+      </c>
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2">
+        <v>2.9213609234904401</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2">
+        <v>2.9454751916308801</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>0.844144991640144</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>3.87466033165438</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>2.9410652439925098</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>2.5455609288272298</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3">
+        <v>3.4772892028063902</v>
+      </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3">
+        <v>2.8158451087685701</v>
+      </c>
+      <c r="M3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3">
+        <v>1.44650071331367</v>
+      </c>
+      <c r="O3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3">
+        <v>2.5531204621314498</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3">
+        <v>2.9035632048670901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4">
+        <v>0.65191429339570495</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>3.03604183141581</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>2.8540332336300098</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <v>1.9190356404840201</v>
+      </c>
+      <c r="I4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>1.4236425627337701</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4">
+        <v>2.8118528717782199</v>
+      </c>
+      <c r="M4" t="s">
+        <v>52</v>
+      </c>
+      <c r="N4">
+        <v>1.1740924061678599</v>
+      </c>
+      <c r="O4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4">
+        <v>2.4985086724130898</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R4">
+        <v>2.8242982518850699</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>0.62071809151104596</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5">
+        <v>2.8258327322600101</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5">
+        <v>1.90936742362418</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5">
+        <v>1.49673332943286</v>
+      </c>
+      <c r="I5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5">
+        <v>0.67545534953947595</v>
+      </c>
+      <c r="K5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5">
+        <v>2.4499844645936499</v>
+      </c>
+      <c r="M5" t="s">
+        <v>51</v>
+      </c>
+      <c r="N5">
+        <v>1.1495265492533</v>
+      </c>
+      <c r="O5" t="s">
+        <v>38</v>
+      </c>
+      <c r="P5">
+        <v>2.11414358208373</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>14</v>
+      </c>
+      <c r="R5">
+        <v>2.7049541557230299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6">
+        <v>0.507893476964282</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6">
+        <v>2.7685214895289199</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6">
+        <v>1.80520563423563</v>
+      </c>
+      <c r="G6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6">
+        <v>1.40190396327322</v>
+      </c>
+      <c r="I6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6">
+        <v>0.57381025112121098</v>
+      </c>
+      <c r="K6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6">
+        <v>2.3698122170202001</v>
+      </c>
+      <c r="M6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6">
+        <v>0.87538276937568904</v>
+      </c>
+      <c r="O6" t="s">
+        <v>51</v>
+      </c>
+      <c r="P6">
+        <v>2.0534245242022999</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R6">
+        <v>2.6626045807406702</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7">
+        <v>9.66955939776383E-2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>2.5736628958694698</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>1.58878531374182</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7">
+        <v>1.2133871868210599</v>
+      </c>
+      <c r="I7" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7">
+        <v>0.50805804815480904</v>
+      </c>
+      <c r="K7" t="s">
+        <v>52</v>
+      </c>
+      <c r="L7">
+        <v>2.31479274349824</v>
+      </c>
+      <c r="M7" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7">
+        <v>0.68170658243239102</v>
+      </c>
+      <c r="O7" t="s">
+        <v>52</v>
+      </c>
+      <c r="P7">
+        <v>1.9848365815544999</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>5</v>
+      </c>
+      <c r="R7">
+        <v>2.4428572206019998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>-0.293175066593657</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8">
+        <v>2.5534247627558599</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8">
+        <v>1.52317274344947</v>
+      </c>
+      <c r="G8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8">
+        <v>0.85518538768278196</v>
+      </c>
+      <c r="I8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J8">
+        <v>0.50153973720139</v>
+      </c>
+      <c r="K8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <v>2.1960424349842298</v>
+      </c>
+      <c r="M8" t="s">
+        <v>36</v>
+      </c>
+      <c r="N8">
+        <v>0.57555500065246601</v>
+      </c>
+      <c r="O8" t="s">
+        <v>5</v>
+      </c>
+      <c r="P8">
+        <v>1.89209128140964</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>19</v>
+      </c>
+      <c r="R8">
+        <v>2.27584198688105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9">
+        <v>-0.32058541912421101</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9">
+        <v>2.2881323427400502</v>
+      </c>
+      <c r="E9" t="s">
+        <v>59</v>
+      </c>
       <c r="F9">
-        <v>-1.0313195608802099</v>
+        <v>1.0648243462575</v>
       </c>
       <c r="G9" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="H9">
-        <v>-1.10809371704752</v>
+        <v>0.84880391507095598</v>
       </c>
       <c r="I9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J9">
-        <v>-2.2317946456383102</v>
+        <v>0.37481496333939801</v>
       </c>
       <c r="K9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="L9">
-        <v>-0.40425202884234102</v>
+        <v>2.0327497987597001</v>
       </c>
       <c r="M9" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="N9">
-        <v>-1.88304138409032</v>
+        <v>0.29987200736231501</v>
       </c>
       <c r="O9" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="P9">
-        <v>-0.77171652121686296</v>
+        <v>1.72761044751419</v>
       </c>
       <c r="Q9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="R9">
-        <v>-0.41031422657414501</v>
+        <v>2.2207035054036002</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2886,55 +3779,55 @@
         <v>47</v>
       </c>
       <c r="B10">
-        <v>-2.2608660055427001</v>
+        <v>-0.54667186416979796</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
       </c>
       <c r="D10">
-        <v>-0.22029910885458201</v>
+        <v>2.2762672078207999</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="F10">
-        <v>-1.1047325807258299</v>
+        <v>1.0487554604562901</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H10">
-        <v>-1.2930716339908801</v>
+        <v>0.82878243440126498</v>
       </c>
       <c r="I10" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="J10">
-        <v>-2.30506603189954</v>
+        <v>0.30384850832987098</v>
       </c>
       <c r="K10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="L10">
-        <v>-0.84219560756351997</v>
+        <v>2.0039036137256199</v>
       </c>
       <c r="M10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N10">
-        <v>-1.9097097710000099</v>
+        <v>0.249132861959865</v>
       </c>
       <c r="O10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="P10">
-        <v>-0.88131336702983498</v>
+        <v>1.68519579335428</v>
       </c>
       <c r="Q10" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="R10">
-        <v>-0.486117235686224</v>
+        <v>1.76624314663329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>